<commit_message>
Completed controllability and severity portion
</commit_message>
<xml_diff>
--- a/Homework/02_HazardAnalysisAndRiskAssessment_Template.xlsx
+++ b/Homework/02_HazardAnalysisAndRiskAssessment_Template.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="272">
   <si>
     <t xml:space="preserve">INSTRUCTIONS:</t>
   </si>
@@ -197,6 +197,18 @@
     <t xml:space="preserve">Driving in the rain is not as common as driving in normal conditions</t>
   </si>
   <si>
+    <t xml:space="preserve">S3 Fatal Injuries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High speed driving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3 Difficult to Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Violent shaking of the steering wheel would be more than most drivers could handle in normal situations</t>
+  </si>
+  <si>
     <t xml:space="preserve">HA-002</t>
   </si>
   <si>
@@ -222,6 +234,12 @@
   </si>
   <si>
     <t xml:space="preserve">Driving on a country road does not happen as often as highway or city driving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2 Normally Controllable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane Keep Assistance cancellation could happen while the vehicle is in a stable condition so transferring control back to the driver would be easy</t>
   </si>
   <si>
     <t xml:space="preserve">HA-003</t>
@@ -1417,8 +1435,8 @@
   </sheetPr>
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12:S13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V13" activeCellId="0" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1432,8 +1450,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="27.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.43"/>
@@ -1886,10 +1904,18 @@
       <c r="P12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
+      <c r="Q12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="R12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="S12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
       <c r="W12" s="14"/>
@@ -1901,16 +1927,16 @@
     </row>
     <row r="13" s="16" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>36</v>
@@ -1921,33 +1947,41 @@
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L13" s="13" t="s">
         <v>41</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="O13" s="13" t="s">
         <v>44</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
+        <v>58</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="R13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="S13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="T13" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
       <c r="W13" s="14"/>
@@ -1959,7 +1993,7 @@
     </row>
     <row r="14" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1991,7 +2025,7 @@
     </row>
     <row r="15" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -2023,7 +2057,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +2085,7 @@
   <dimension ref="A1:Z110"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R12:S13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2084,7 +2118,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -2171,16 +2205,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
@@ -2211,10 +2245,10 @@
         <v>OM01</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D5" s="26" t="str">
         <f aca="false">$A5 &amp; " - " &amp; $B5</f>
@@ -2249,10 +2283,10 @@
         <v>OM02</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D6" s="26" t="str">
         <f aca="false">$A6 &amp; " - " &amp; $B6</f>
@@ -2287,10 +2321,10 @@
         <v>OM03</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D7" s="26" t="str">
         <f aca="false">$A7 &amp; " - " &amp; $B7</f>
@@ -2325,10 +2359,10 @@
         <v>OM04</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D8" s="26" t="str">
         <f aca="false">$A8 &amp; " - " &amp; $B8</f>
@@ -2363,10 +2397,10 @@
         <v>OM05</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D9" s="26" t="str">
         <f aca="false">$A9 &amp; " - " &amp; $B9</f>
@@ -2401,10 +2435,10 @@
         <v>OM06</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D10" s="26" t="str">
         <f aca="false">$A10 &amp; " - " &amp; $B10</f>
@@ -2439,10 +2473,10 @@
         <v>OM07</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D11" s="26" t="str">
         <f aca="false">$A11 &amp; " - " &amp; $B11</f>
@@ -2477,10 +2511,10 @@
         <v>OM08</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D12" s="26" t="str">
         <f aca="false">$A12 &amp; " - " &amp; $B12</f>
@@ -2515,10 +2549,10 @@
         <v>OM09</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D13" s="26" t="str">
         <f aca="false">$A13 &amp; " - " &amp; $B13</f>
@@ -2635,16 +2669,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
@@ -2675,10 +2709,10 @@
         <v>OS01</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D18" s="26" t="str">
         <f aca="false">$A18 &amp; " - " &amp; $B18</f>
@@ -2713,10 +2747,10 @@
         <v>OS02</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D19" s="26" t="str">
         <f aca="false">$A19 &amp; " - " &amp; $B19</f>
@@ -2751,10 +2785,10 @@
         <v>OS03</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D20" s="26" t="str">
         <f aca="false">$A20 &amp; " - " &amp; $B20</f>
@@ -2792,7 +2826,7 @@
         <v>34</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D21" s="26" t="str">
         <f aca="false">$A21 &amp; " - " &amp; $B21</f>
@@ -2827,10 +2861,10 @@
         <v>OS05</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D22" s="26" t="str">
         <f aca="false">$A22 &amp; " - " &amp; $B22</f>
@@ -2865,10 +2899,10 @@
         <v>OS06</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D23" s="26" t="str">
         <f aca="false">$A23 &amp; " - " &amp; $B23</f>
@@ -2903,10 +2937,10 @@
         <v>OS07</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D24" s="26" t="str">
         <f aca="false">$A24 &amp; " - " &amp; $B24</f>
@@ -2941,10 +2975,10 @@
         <v>OS08</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D25" s="26" t="str">
         <f aca="false">$A25 &amp; " - " &amp; $B25</f>
@@ -2979,10 +3013,10 @@
         <v>OS09</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D26" s="26" t="str">
         <f aca="false">$A26 &amp; " - " &amp; $B26</f>
@@ -3017,10 +3051,10 @@
         <v>OS10</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D27" s="26" t="str">
         <f aca="false">$A27 &amp; " - " &amp; $B27</f>
@@ -3055,10 +3089,10 @@
         <v>OS11</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D28" s="26" t="str">
         <f aca="false">$A28 &amp; " - " &amp; $B28</f>
@@ -3175,16 +3209,16 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
@@ -3215,10 +3249,10 @@
         <v>SD01</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D33" s="26" t="str">
         <f aca="false">$A33 &amp; " - " &amp; $B33</f>
@@ -3253,10 +3287,10 @@
         <v>SD02</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D34" s="26" t="str">
         <f aca="false">$A34 &amp; " - " &amp; $B34</f>
@@ -3291,10 +3325,10 @@
         <v>SD03</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D35" s="26" t="str">
         <f aca="false">$A35 &amp; " - " &amp; $B35</f>
@@ -3329,10 +3363,10 @@
         <v>SD04</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D36" s="26" t="str">
         <f aca="false">$A36 &amp; " - " &amp; $B36</f>
@@ -3367,10 +3401,10 @@
         <v>SD05</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D37" s="26" t="str">
         <f aca="false">$A37 &amp; " - " &amp; $B37</f>
@@ -3405,10 +3439,10 @@
         <v>SD06</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D38" s="26" t="str">
         <f aca="false">$A38 &amp; " - " &amp; $B38</f>
@@ -3443,10 +3477,10 @@
         <v>SD07</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D39" s="26" t="str">
         <f aca="false">$A39 &amp; " - " &amp; $B39</f>
@@ -3533,7 +3567,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="21" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
@@ -3563,16 +3597,16 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
@@ -3603,10 +3637,10 @@
         <v>IU01</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D44" s="26" t="str">
         <f aca="false">$A44 &amp; " - " &amp; $B44</f>
@@ -3641,10 +3675,10 @@
         <v>IU02</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D45" s="26" t="str">
         <f aca="false">$A45 &amp; " - " &amp; $B45</f>
@@ -3679,10 +3713,10 @@
         <v>IU03</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D46" s="26" t="str">
         <f aca="false">$A46 &amp; " - " &amp; $B46</f>
@@ -3799,16 +3833,16 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
@@ -3839,10 +3873,10 @@
         <v>EN01</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D51" s="26" t="str">
         <f aca="false">$A51 &amp; " - " &amp; $B51</f>
@@ -3877,10 +3911,10 @@
         <v>EN02</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D52" s="26" t="str">
         <f aca="false">$A52 &amp; " - " &amp; $B52</f>
@@ -3915,10 +3949,10 @@
         <v>EN03</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D53" s="26" t="str">
         <f aca="false">$A53 &amp; " - " &amp; $B53</f>
@@ -3953,10 +3987,10 @@
         <v>EN04</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D54" s="26" t="str">
         <f aca="false">$A54 &amp; " - " &amp; $B54</f>
@@ -3991,10 +4025,10 @@
         <v>EN05</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D55" s="26" t="str">
         <f aca="false">$A55 &amp; " - " &amp; $B55</f>
@@ -4032,7 +4066,7 @@
         <v>35</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D56" s="26" t="str">
         <f aca="false">$A56 &amp; " - " &amp; $B56</f>
@@ -4067,10 +4101,10 @@
         <v>EN07</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D57" s="26" t="str">
         <f aca="false">$A57 &amp; " - " &amp; $B57</f>
@@ -4105,10 +4139,10 @@
         <v>EN08</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D58" s="26" t="str">
         <f aca="false">$A58 &amp; " - " &amp; $B58</f>
@@ -4143,10 +4177,10 @@
         <v>EN09</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D59" s="26" t="str">
         <f aca="false">$A59 &amp; " - " &amp; $B59</f>
@@ -5126,7 +5160,7 @@
   <dimension ref="A1:AC19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T6" activeCellId="1" sqref="R12:S13 T6"/>
+      <selection pane="topLeft" activeCell="T6" activeCellId="0" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5191,7 +5225,7 @@
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="28"/>
       <c r="B2" s="29" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -5297,7 +5331,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>15</v>
@@ -5312,7 +5346,7 @@
         <v>18</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>20</v>
@@ -5366,64 +5400,64 @@
         <v>33</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="M6" s="34" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="N6" s="34" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="O6" s="34" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="P6" s="34" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="Q6" s="34" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="R6" s="34" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="S6" s="34" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="T6" s="34" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="V6" s="34" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="W6" s="35" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="X6" s="17"/>
       <c r="Y6" s="17"/>
@@ -5528,7 +5562,7 @@
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20"/>
       <c r="B10" s="29" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -5594,7 +5628,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -5641,7 +5675,7 @@
         <v>13</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>15</v>
@@ -5656,7 +5690,7 @@
         <v>18</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>20</v>
@@ -5706,67 +5740,67 @@
         <v>32</v>
       </c>
       <c r="C14" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="K14" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="L14" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="M14" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="N14" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="O14" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="P14" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q14" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="R14" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="S14" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="T14" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="U14" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="V14" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="F14" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="I14" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="J14" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="K14" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="L14" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="M14" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="N14" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="O14" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="P14" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q14" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="R14" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="S14" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="T14" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="U14" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="V14" s="34" t="s">
-        <v>130</v>
-      </c>
       <c r="W14" s="35" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="X14" s="17"/>
       <c r="Y14" s="17"/>
@@ -5777,70 +5811,70 @@
     </row>
     <row r="15" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="34" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E15" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="H15" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="F15" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="G15" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="H15" s="34" t="s">
-        <v>138</v>
-      </c>
       <c r="I15" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="K15" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="J15" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="K15" s="34" t="s">
-        <v>140</v>
-      </c>
       <c r="L15" s="34" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="M15" s="34" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="O15" s="34" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="P15" s="34" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="Q15" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="R15" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="S15" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="R15" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="S15" s="34" t="s">
-        <v>142</v>
-      </c>
       <c r="T15" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="U15" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="V15" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="W15" s="35" t="s">
         <v>149</v>
-      </c>
-      <c r="U15" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="V15" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="W15" s="35" t="s">
-        <v>143</v>
       </c>
       <c r="X15" s="17"/>
       <c r="Y15" s="17"/>
@@ -5851,70 +5885,70 @@
     </row>
     <row r="16" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="34" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E16" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="F16" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>138</v>
-      </c>
       <c r="I16" s="34" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="L16" s="34" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="M16" s="34" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="O16" s="34" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="P16" s="34" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="Q16" s="34" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="R16" s="34" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="S16" s="34" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="T16" s="34" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="U16" s="34" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="V16" s="34" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="W16" s="35" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="X16" s="17"/>
       <c r="Y16" s="17"/>
@@ -5925,70 +5959,70 @@
     </row>
     <row r="17" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="34" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F17" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="K17" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="L17" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="N17" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="O17" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="P17" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q17" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="R17" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="G17" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="I17" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="J17" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="K17" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="L17" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="M17" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="N17" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="O17" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="P17" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q17" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="R17" s="34" t="s">
-        <v>158</v>
-      </c>
       <c r="S17" s="34" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="T17" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="U17" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="V17" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="W17" s="35" t="s">
         <v>149</v>
-      </c>
-      <c r="U17" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="V17" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="W17" s="35" t="s">
-        <v>143</v>
       </c>
       <c r="X17" s="17"/>
       <c r="Y17" s="17"/>
@@ -5999,70 +6033,70 @@
     </row>
     <row r="18" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="34" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E18" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="H18" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="F18" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>138</v>
-      </c>
       <c r="I18" s="34" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="J18" s="34" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="L18" s="34" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="M18" s="34" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="N18" s="34" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="O18" s="34" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="P18" s="34" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="Q18" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="R18" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="S18" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="R18" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="S18" s="34" t="s">
-        <v>170</v>
-      </c>
       <c r="T18" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="U18" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="U18" s="34" t="s">
-        <v>171</v>
-      </c>
       <c r="V18" s="34" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="W18" s="35" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="X18" s="17"/>
       <c r="Y18" s="17"/>
@@ -6980,7 +7014,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R12:S13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7022,7 +7056,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -7052,16 +7086,16 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="37"/>
@@ -7092,10 +7126,10 @@
         <v>DV01</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D4" s="26" t="str">
         <f aca="false">$A4 &amp; " - " &amp; $B4</f>
@@ -7130,10 +7164,10 @@
         <v>DV02</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D5" s="26" t="str">
         <f aca="false">$A5 &amp; " - " &amp; $B5</f>
@@ -7168,10 +7202,10 @@
         <v>DV03</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D6" s="26" t="str">
         <f aca="false">$A6 &amp; " - " &amp; $B6</f>
@@ -7209,7 +7243,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D7" s="26" t="str">
         <f aca="false">$A7 &amp; " - " &amp; $B7</f>
@@ -7244,10 +7278,10 @@
         <v>DV05</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D8" s="26" t="str">
         <f aca="false">$A8 &amp; " - " &amp; $B8</f>
@@ -7282,10 +7316,10 @@
         <v>DV06</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D9" s="26" t="str">
         <f aca="false">$A9 &amp; " - " &amp; $B9</f>
@@ -7320,10 +7354,10 @@
         <v>DV07</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D10" s="26" t="str">
         <f aca="false">$A10 &amp; " - " &amp; $B10</f>
@@ -7358,10 +7392,10 @@
         <v>DV08</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D11" s="26" t="str">
         <f aca="false">$A11 &amp; " - " &amp; $B11</f>
@@ -7396,10 +7430,10 @@
         <v>DV09</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D12" s="26" t="str">
         <f aca="false">$A12 &amp; " - " &amp; $B12</f>
@@ -7434,10 +7468,10 @@
         <v>DV10</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D13" s="26" t="str">
         <f aca="false">$A13 &amp; " - " &amp; $B13</f>
@@ -7472,10 +7506,10 @@
         <v>DV11</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D14" s="26" t="str">
         <f aca="false">$A14 &amp; " - " &amp; $B14</f>
@@ -7510,10 +7544,10 @@
         <v>DV12</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D15" s="26" t="str">
         <f aca="false">$A15 &amp; " - " &amp; $B15</f>
@@ -7548,10 +7582,10 @@
         <v>DV13</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D16" s="26" t="str">
         <f aca="false">$A16 &amp; " - " &amp; $B16</f>
@@ -7586,10 +7620,10 @@
         <v>DV14</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D17" s="26" t="str">
         <f aca="false">$A17 &amp; " - " &amp; $B17</f>
@@ -7624,10 +7658,10 @@
         <v>DV15</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D18" s="26" t="str">
         <f aca="false">$A18 &amp; " - " &amp; $B18</f>
@@ -7662,10 +7696,10 @@
         <v>DV16</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D19" s="26" t="str">
         <f aca="false">$A19 &amp; " - " &amp; $B19</f>
@@ -7700,10 +7734,10 @@
         <v>DV17</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D20" s="26" t="str">
         <f aca="false">$A20 &amp; " - " &amp; $B20</f>
@@ -7738,10 +7772,10 @@
         <v>DV18</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D21" s="26" t="str">
         <f aca="false">$A21 &amp; " - " &amp; $B21</f>
@@ -7776,10 +7810,10 @@
         <v>DV19</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D22" s="26" t="str">
         <f aca="false">$A22 &amp; " - " &amp; $B22</f>
@@ -7814,10 +7848,10 @@
         <v>DV20</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D23" s="26" t="str">
         <f aca="false">$A23 &amp; " - " &amp; $B23</f>
@@ -7904,7 +7938,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40"/>
@@ -7934,16 +7968,16 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E27" s="37"/>
       <c r="F27" s="37"/>
@@ -7974,7 +8008,7 @@
         <v>EV-07</v>
       </c>
       <c r="B28" s="44" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C28" s="45"/>
       <c r="D28" s="46" t="str">
@@ -8010,7 +8044,7 @@
         <v>EV-06</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C29" s="45"/>
       <c r="D29" s="46" t="str">
@@ -8046,7 +8080,7 @@
         <v>EV-05</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C30" s="45"/>
       <c r="D30" s="46" t="str">
@@ -8082,7 +8116,7 @@
         <v>EV-04</v>
       </c>
       <c r="B31" s="44" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C31" s="45"/>
       <c r="D31" s="46" t="str">
@@ -8118,7 +8152,7 @@
         <v>EV-03</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C32" s="45"/>
       <c r="D32" s="46" t="str">
@@ -8154,7 +8188,7 @@
         <v>EV-02</v>
       </c>
       <c r="B33" s="44" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C33" s="45"/>
       <c r="D33" s="46" t="str">
@@ -8190,7 +8224,7 @@
         <v>EV-01</v>
       </c>
       <c r="B34" s="44" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C34" s="45"/>
       <c r="D34" s="46" t="str">
@@ -8262,7 +8296,7 @@
         <v>EV01</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C36" s="45"/>
       <c r="D36" s="46" t="str">
@@ -8298,7 +8332,7 @@
         <v>EV02</v>
       </c>
       <c r="B37" s="44" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C37" s="45"/>
       <c r="D37" s="46" t="str">
@@ -8334,7 +8368,7 @@
         <v>EV03</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C38" s="45"/>
       <c r="D38" s="46" t="str">
@@ -8370,7 +8404,7 @@
         <v>EV04</v>
       </c>
       <c r="B39" s="44" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C39" s="45"/>
       <c r="D39" s="46" t="str">
@@ -8406,7 +8440,7 @@
         <v>EV05</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C40" s="45"/>
       <c r="D40" s="46" t="str">
@@ -8442,7 +8476,7 @@
         <v>EV06</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C41" s="45"/>
       <c r="D41" s="46" t="str">
@@ -8520,7 +8554,7 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="1" sqref="R12:S13 E22"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8534,7 +8568,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -8564,19 +8598,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
@@ -8602,10 +8636,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="49" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
@@ -8637,16 +8671,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="E4" s="26" t="str">
         <f aca="false">$A4 &amp; " - " &amp; $B4</f>
@@ -8676,16 +8710,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="49" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="E5" s="26" t="str">
         <f aca="false">$A5 &amp; " - " &amp; $B5</f>
@@ -8715,16 +8749,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="E6" s="26" t="str">
         <f aca="false">$A6 &amp; " - " &amp; $B6</f>
@@ -8754,16 +8788,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="49" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E7" s="26" t="str">
         <f aca="false">$A7 &amp; " - " &amp; $B7</f>
@@ -8849,7 +8883,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -8879,19 +8913,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -8917,16 +8951,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="49" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E12" s="26" t="str">
         <f aca="false">$A12 &amp; " - " &amp; $B12</f>
@@ -8956,16 +8990,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="49" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E13" s="26" t="str">
         <f aca="false">$A13 &amp; " - " &amp; $B13</f>
@@ -8995,16 +9029,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="49" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="E14" s="26" t="str">
         <f aca="false">$A14 &amp; " - " &amp; $B14</f>
@@ -9034,16 +9068,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="49" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="E15" s="26" t="str">
         <f aca="false">$A15 &amp; " - " &amp; $B15</f>
@@ -9129,7 +9163,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="21" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -9159,17 +9193,17 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D19" s="51"/>
       <c r="E19" s="23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
@@ -9195,13 +9229,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="49" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D20" s="53"/>
       <c r="E20" s="26" t="str">
@@ -9232,13 +9266,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="49" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="D21" s="53"/>
       <c r="E21" s="26" t="str">
@@ -9269,13 +9303,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="49" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D22" s="53"/>
       <c r="E22" s="26" t="str">
@@ -9306,13 +9340,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="49" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="D23" s="53"/>
       <c r="E23" s="26" t="str">
@@ -9388,7 +9422,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="1" sqref="R12:S13 D15"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9398,13 +9432,13 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="56" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="E2" s="58"/>
       <c r="F2" s="58"/>
@@ -9414,238 +9448,238 @@
       <c r="B3" s="56"/>
       <c r="C3" s="57"/>
       <c r="D3" s="45" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="59" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G4" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="59"/>
       <c r="C5" s="60" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F5" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G5" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="59"/>
       <c r="C6" s="60" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G6" s="60" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="59"/>
       <c r="C7" s="60" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F7" s="60" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G7" s="60" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="59" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C8" s="60" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="D8" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F8" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G8" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="59"/>
       <c r="C9" s="60" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D9" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F9" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G9" s="60" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="59"/>
       <c r="C10" s="60" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D10" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F10" s="60" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G10" s="60" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="59"/>
       <c r="C11" s="60" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D11" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E11" s="60" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F11" s="60" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="G11" s="60" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="59" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="D12" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E12" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F12" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G12" s="60" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="59"/>
       <c r="C13" s="60" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D13" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E13" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F13" s="60" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G13" s="60" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="59"/>
       <c r="C14" s="60" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E14" s="60" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F14" s="60" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="G14" s="60" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="59"/>
       <c r="C15" s="60" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D15" s="60" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E15" s="60" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="F15" s="60" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="G15" s="60" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move repository Add Additional answers to blanks
</commit_message>
<xml_diff>
--- a/Homework/02_HazardAnalysisAndRiskAssessment_Template.xlsx
+++ b/Homework/02_HazardAnalysisAndRiskAssessment_Template.xlsx
@@ -1498,8 +1498,8 @@
   </sheetPr>
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V12" activeCellId="0" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1514,7 +1514,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="27.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.43"/>
@@ -1523,8 +1523,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="40.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="14.43"/>
   </cols>
   <sheetData>

</xml_diff>